<commit_message>
Nuevos materiales. Fin de primer cuatrimestre
</commit_message>
<xml_diff>
--- a/Simulacion/Método del rechazo Excel.xlsx
+++ b/Simulacion/Método del rechazo Excel.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\OneDrive\Docencia\Simulacion\2020\Clase 200413\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f22b094dc322757/Docencia/Simulacion/2020/Clase 200406/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{97B0F4BC-0AFF-44EF-AB4E-D0C7F1F77208}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{245F2A31-C893-4800-B5A9-AF36212BC329}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="8_{1FAACEA5-625F-417C-8E10-2E4C7C9E4BA5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{05E39E7A-72DA-4D10-8AD1-F3C7A47ADC9B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{04C9D087-CF0C-4B34-8919-DAEE78BC6236}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{04C9D087-CF0C-4B34-8919-DAEE78BC6236}"/>
   </bookViews>
   <sheets>
     <sheet name="Ejemplo 3" sheetId="1" r:id="rId1"/>
-    <sheet name="Ejemplo 1" sheetId="2" r:id="rId2"/>
-    <sheet name="Ejemplo 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Ejemplo 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Ejemplo 1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -769,8 +769,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.6631889763779528E-2"/>
-          <c:y val="3.7037037037037035E-2"/>
+          <c:x val="9.9652230971128599E-3"/>
+          <c:y val="4.1666666666666664E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -813,7 +813,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ejemplo 1'!$B$2</c:f>
+              <c:f>'Ejemplo 2'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -836,7 +836,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Ejemplo 1'!$A$3:$A$13</c:f>
+              <c:f>'Ejemplo 2'!$A$3:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -878,7 +878,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Ejemplo 1'!$B$3:$B$13</c:f>
+              <c:f>'Ejemplo 2'!$B$3:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1152,7 +1152,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ejemplo 2'!$B$1</c:f>
+              <c:f>'Ejemplo 1'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1175,7 +1175,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Ejemplo 2'!$A$2:$A$42</c:f>
+              <c:f>'Ejemplo 1'!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -1307,7 +1307,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Ejemplo 2'!$B$2:$B$42</c:f>
+              <c:f>'Ejemplo 1'!$B$2:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -3349,50 +3349,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>584728</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>12997</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F126AC58-1EB8-4647-8EEE-D13330C66DFD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2108200" y="3765550"/>
-          <a:ext cx="6096528" cy="3429297"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3400,16 +3356,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>460375</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>730250</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>460375</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3434,50 +3390,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>641350</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>52388</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30CF0389-44B2-4CC6-90C1-E1241658112E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1733550" y="0"/>
-          <a:ext cx="5003800" cy="2814638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3485,16 +3397,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3517,50 +3429,6 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>120651</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>165895</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9BCA8A7-7BB8-4034-8201-F77AF0304481}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1733550" y="857251"/>
-          <a:ext cx="4991100" cy="2807494"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3865,8 +3733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1C3795-E9F7-42A7-BBE3-EBBBB0D97DA8}">
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4723,7 +4591,7 @@
   <dimension ref="A2:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5320,8 +5188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D7407F-EF5D-469E-97EF-DB3672D3114B}">
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5396,12 +5264,12 @@
         <v>1.052525977369841</v>
       </c>
       <c r="N3" s="12">
-        <f>(3/2)*M3-(3/4)*M3^2</f>
-        <v>0.74793076627600708</v>
+        <f>(3/2)*M3-(3/4)*K3^2</f>
+        <v>1.3710744161100727</v>
       </c>
       <c r="O3" s="12">
         <f>N3/$I$4</f>
-        <v>0.99724102170134277</v>
+        <v>1.8280992214800971</v>
       </c>
       <c r="P3" s="12" t="str">
         <f t="shared" ref="P3:P19" si="1">IF(L3&lt;O3,"ACEPTO x","RECHAZO x")</f>
@@ -5437,12 +5305,12 @@
         <v>0.50805092066115987</v>
       </c>
       <c r="N4" s="12">
-        <f t="shared" ref="N4:N19" si="3">(3/2)*M4-(3/4)*M4^2</f>
-        <v>0.56848957750325069</v>
+        <f t="shared" ref="N4:N19" si="3">(3/2)*M4-(3/4)*K4^2</f>
+        <v>0.71367968011961747</v>
       </c>
       <c r="O4" s="12">
         <f t="shared" ref="O4:O19" si="4">N4/$I$4</f>
-        <v>0.75798610333766758</v>
+        <v>0.95157290682615658</v>
       </c>
       <c r="P4" s="12" t="str">
         <f t="shared" si="1"/>
@@ -5472,11 +5340,11 @@
       </c>
       <c r="N5" s="10">
         <f t="shared" si="3"/>
-        <v>5.2662270673921513E-2</v>
+        <v>5.3381064535366181E-2</v>
       </c>
       <c r="O5" s="10">
         <f t="shared" si="4"/>
-        <v>7.0216360898562022E-2</v>
+        <v>7.1174752713821579E-2</v>
       </c>
       <c r="P5" s="10" t="str">
         <f t="shared" si="1"/>
@@ -5506,11 +5374,11 @@
       </c>
       <c r="N6" s="12">
         <f t="shared" si="3"/>
-        <v>0.73764371087961267</v>
+        <v>1.4538105049029888</v>
       </c>
       <c r="O6" s="12">
         <f t="shared" si="4"/>
-        <v>0.98352494783948352</v>
+        <v>1.9384140065373183</v>
       </c>
       <c r="P6" s="12" t="str">
         <f t="shared" si="1"/>
@@ -5540,11 +5408,11 @@
       </c>
       <c r="N7" s="12">
         <f t="shared" si="3"/>
-        <v>0.74101648320725821</v>
+        <v>1.187129449887526</v>
       </c>
       <c r="O7" s="12">
         <f t="shared" si="4"/>
-        <v>0.98802197760967758</v>
+        <v>1.5828392665167013</v>
       </c>
       <c r="P7" s="12" t="str">
         <f t="shared" si="1"/>
@@ -5574,11 +5442,11 @@
       </c>
       <c r="N8" s="12">
         <f t="shared" si="3"/>
-        <v>0.52601161491792703</v>
+        <v>0.64170179782123915</v>
       </c>
       <c r="O8" s="12">
         <f t="shared" si="4"/>
-        <v>0.70134881989056941</v>
+        <v>0.85560239709498553</v>
       </c>
       <c r="P8" s="12" t="str">
         <f t="shared" si="1"/>
@@ -5608,11 +5476,11 @@
       </c>
       <c r="N9" s="12">
         <f t="shared" si="3"/>
-        <v>0.3491972446376343</v>
+        <v>0.38989147457588469</v>
       </c>
       <c r="O9" s="12">
         <f t="shared" si="4"/>
-        <v>0.46559632618351238</v>
+        <v>0.51985529943451292</v>
       </c>
       <c r="P9" s="12" t="str">
         <f t="shared" si="1"/>
@@ -5642,11 +5510,11 @@
       </c>
       <c r="N10" s="10">
         <f t="shared" si="3"/>
-        <v>0.1323402550360212</v>
+        <v>0.13715371463374987</v>
       </c>
       <c r="O10" s="10">
         <f t="shared" si="4"/>
-        <v>0.17645367338136161</v>
+        <v>0.1828716195116665</v>
       </c>
       <c r="P10" s="10" t="str">
         <f t="shared" si="1"/>
@@ -5676,15 +5544,15 @@
       </c>
       <c r="N11" s="12">
         <f t="shared" si="3"/>
-        <v>7.1195984195918438E-2</v>
+        <v>2.2130708197785349</v>
       </c>
       <c r="O11" s="12">
         <f t="shared" si="4"/>
-        <v>9.4927978927891246E-2</v>
+        <v>2.9507610930380466</v>
       </c>
       <c r="P11" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>RECHAZO x</v>
+        <v>ACEPTO x</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
@@ -5710,11 +5578,11 @@
       </c>
       <c r="N12" s="12">
         <f t="shared" si="3"/>
-        <v>0.56073887243235254</v>
+        <v>1.8303202352810979</v>
       </c>
       <c r="O12" s="12">
         <f t="shared" si="4"/>
-        <v>0.74765182990980339</v>
+        <v>2.4404269803747973</v>
       </c>
       <c r="P12" s="12" t="str">
         <f t="shared" si="1"/>
@@ -5742,13 +5610,13 @@
         <f t="shared" si="2"/>
         <v>1.1842876154416953</v>
       </c>
-      <c r="N13" s="12">
+      <c r="N13" s="13">
         <f t="shared" si="3"/>
-        <v>0.72452855609611033</v>
+        <v>1.5134557063959346</v>
       </c>
       <c r="O13" s="13">
         <f t="shared" si="4"/>
-        <v>0.96603807479481374</v>
+        <v>2.0179409418612462</v>
       </c>
       <c r="P13" s="13" t="str">
         <f t="shared" si="1"/>
@@ -5776,13 +5644,13 @@
         <f t="shared" si="2"/>
         <v>1.1564031366424534</v>
       </c>
-      <c r="N14" s="12">
+      <c r="N14" s="13">
         <f t="shared" si="3"/>
-        <v>0.73165354413630146</v>
+        <v>1.4838669147568355</v>
       </c>
       <c r="O14" s="13">
         <f t="shared" si="4"/>
-        <v>0.97553805884840195</v>
+        <v>1.9784892196757806</v>
       </c>
       <c r="P14" s="13" t="str">
         <f t="shared" si="1"/>
@@ -5810,13 +5678,13 @@
         <f t="shared" si="2"/>
         <v>0.78530641510693178</v>
       </c>
-      <c r="N15" s="12">
+      <c r="N15" s="13">
         <f t="shared" si="3"/>
-        <v>0.7154299984543222</v>
+        <v>1.0623272166088789</v>
       </c>
       <c r="O15" s="13">
         <f t="shared" si="4"/>
-        <v>0.9539066646057629</v>
+        <v>1.4164362888118385</v>
       </c>
       <c r="P15" s="13" t="str">
         <f t="shared" si="1"/>
@@ -5844,13 +5712,13 @@
         <f t="shared" si="2"/>
         <v>1.05116524611733</v>
       </c>
-      <c r="N16" s="12">
+      <c r="N16" s="13">
         <f t="shared" si="3"/>
-        <v>0.74803658819231467</v>
+        <v>1.3695700489300748</v>
       </c>
       <c r="O16" s="13">
         <f t="shared" si="4"/>
-        <v>0.99738211758975293</v>
+        <v>1.8260933985734331</v>
       </c>
       <c r="P16" s="13" t="str">
         <f t="shared" si="1"/>
@@ -5878,13 +5746,13 @@
         <f t="shared" si="2"/>
         <v>0.22560300771466291</v>
       </c>
-      <c r="N17" s="12">
+      <c r="N17" s="13">
         <f t="shared" si="3"/>
-        <v>0.30023197375456767</v>
+        <v>0.32886137711763769</v>
       </c>
       <c r="O17" s="13">
         <f t="shared" si="4"/>
-        <v>0.40030929833942358</v>
+        <v>0.43848183615685027</v>
       </c>
       <c r="P17" s="13" t="str">
         <f t="shared" si="1"/>
@@ -5912,17 +5780,17 @@
         <f t="shared" si="2"/>
         <v>0.30364774659946003</v>
       </c>
-      <c r="N18" s="12">
+      <c r="N18" s="13">
         <f t="shared" si="3"/>
-        <v>0.38632015438799261</v>
+        <v>0.43818375352139072</v>
       </c>
       <c r="O18" s="13">
         <f t="shared" si="4"/>
-        <v>0.51509353918399015</v>
+        <v>0.58424500469518759</v>
       </c>
       <c r="P18" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>RECHAZO x</v>
+        <v>ACEPTO x</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
@@ -5946,13 +5814,13 @@
         <f t="shared" si="2"/>
         <v>1.071952805621039</v>
       </c>
-      <c r="N19" s="12">
+      <c r="N19" s="13">
         <f t="shared" si="3"/>
-        <v>0.74611709532244586</v>
+        <v>1.3924761801542804</v>
       </c>
       <c r="O19" s="13">
         <f t="shared" si="4"/>
-        <v>0.9948227937632611</v>
+        <v>1.856634906872374</v>
       </c>
       <c r="P19" s="13" t="str">
         <f t="shared" si="1"/>

</xml_diff>